<commit_message>
AllShows class and test cases added to the project
</commit_message>
<xml_diff>
--- a/nbc/testData/FooterLinkName.xlsx
+++ b/nbc/testData/FooterLinkName.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maruf/AllJavaProject/AutomationP1/nbc/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE11CFA0-EFFD-C147-B9A4-BFF084F042D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069609DE-A829-A147-B241-0018A0B89466}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33580" yWindow="-80" windowWidth="23660" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="1840" windowWidth="23660" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>SHARE THE MOMENT™</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>Video Viewing Policy</t>
+  </si>
+  <si>
+    <t>WebElementName</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>efd</t>
   </si>
 </sst>
 </file>
@@ -89,6 +101,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -438,11 +451,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -451,95 +462,108 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Xls and xlsx reader updated
</commit_message>
<xml_diff>
--- a/nbc/testData/FooterLinkName.xlsx
+++ b/nbc/testData/FooterLinkName.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maruf/AllJavaProject/AutomationP1/nbc/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069609DE-A829-A147-B241-0018A0B89466}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB2B349-2ED2-2C4E-AF5A-1BBB2F2F410C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1840" windowWidth="23660" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36780" yWindow="780" windowWidth="23660" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>Casting</t>
   </si>
   <si>
-    <t>NBC Store</t>
-  </si>
-  <si>
     <t>Parental Guidelines and TV Ratings</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>efd</t>
+  </si>
+  <si>
+    <t>Tickets and NBC Studio Tour</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,9 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -462,10 +464,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -473,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -484,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -504,67 +506,67 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>